<commit_message>
Correzione XML e JSON
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111TOPGATEXXXX/topgate/skipper/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111TOPGATEXXXX/topgate/skipper/1.0/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elia\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F5CF66-1A70-4209-8BC1-386F06236E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F7FC6F-F3EF-4FB6-997B-B4B52F7C00A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="331">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -967,6 +967,336 @@
   </si>
   <si>
     <t>subject_application_version:  1.0</t>
+  </si>
+  <si>
+    <t>Segnalato all'utente e su log di sistema</t>
+  </si>
+  <si>
+    <t>Salvataggio dei documenti prodotti su DB e segnalazione errore</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Certificato Vaccinale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2023-06-06T14:06:10+00:00</t>
+  </si>
+  <si>
+    <t>40c6d620c01ab39a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.9bf750de30^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Certificato Vaccinale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2023-06-06T14:06:59+00:00</t>
+  </si>
+  <si>
+    <t>066665575e7d6464</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.31d006c495^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Certificato Vaccinale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2023-06-06T14:07:29+00:00</t>
+  </si>
+  <si>
+    <t>2c460b1311a71f7a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.5868207c1b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Certificato Vaccinale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2023-06-06T14:08:03+00:00</t>
+  </si>
+  <si>
+    <t>47ac2f953953c692</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.2db33999b6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_TOKEN_JWT_CERT_VAC_KO</t>
+  </si>
+  <si>
+    <t>2023-06-06T14:22:02+00:00</t>
+  </si>
+  <si>
+    <t>689f600b08ad0fa9</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_TOKEN_JWT_CAMPO_CERT_VAC_KO</t>
+  </si>
+  <si>
+    <t>2023-06-06T14:24:15+00:00</t>
+  </si>
+  <si>
+    <t>8a6db0fc31f11786</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CERT_VAC_TIMEOUT</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT5_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2023-06-06T14:26:36+00:00</t>
+  </si>
+  <si>
+    <t>5615f038ea95218c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.75c7ba1cde^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT6_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2023-06-06T14:29:00+00:00</t>
+  </si>
+  <si>
+    <t>3fd1e4a3162608f8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.337387c473^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT7_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2023-06-06T14:30:39+00:00</t>
+  </si>
+  <si>
+    <t>df90246cc8583e8a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.f92e843f53^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT8_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2023-06-06T14:31:19+00:00</t>
+  </si>
+  <si>
+    <t>7ca2d24a0fcd0dc1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.d145185cae^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT9_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2023-06-06T14:31:45+00:00</t>
+  </si>
+  <si>
+    <t>ddcce3fd35ea2ede</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.feb15d4b48^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT10_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2023-06-06T14:32:21+00:00</t>
+  </si>
+  <si>
+    <t>808333f1c8668240</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.e271c1bb43^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT11_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2023-06-06T14:32:46+00:00</t>
+  </si>
+  <si>
+    <t>dd9d6f873d3f4efe</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.0b92872779^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT12_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2023-06-06T14:33:21+00:00</t>
+  </si>
+  <si>
+    <t>6c369f97af511f4e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.bc40f9c721^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT13_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2023-06-06T14:33:49+00:00</t>
+  </si>
+  <si>
+    <t>4ab13c36a7bf7b1c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.0ee023f578^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT14_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2023-06-06T14:34:26+00:00</t>
+  </si>
+  <si>
+    <t>cec556b1cb132542</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.0e41728773^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT15_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2023-06-06T14:34:51+00:00</t>
+  </si>
+  <si>
+    <t>56f036f42037c159</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.594b34f52a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT16_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2023-06-06T14:35:31+00:00</t>
+  </si>
+  <si>
+    <t>ff81a15438f56572</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.e9567b2448^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT17_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2023-06-06T14:36:02+00:00</t>
+  </si>
+  <si>
+    <t>8af51512c2e88b9c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.09b38861ca^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Certificato Vaccinale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 0" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2023-06-15T06:54:18+00:00</t>
+  </si>
+  <si>
+    <t>de722e732d8a610e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.b22926dcf3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1295,7 +1625,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1387,6 +1717,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3866,13 +4199,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:T649"/>
+  <dimension ref="A1:T629"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="L29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="Q35" sqref="Q35"/>
+      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3910,12 +4243,12 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="38"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -3933,14 +4266,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="45" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="46" t="s">
         <v>229</v>
       </c>
-      <c r="D3" s="37"/>
+      <c r="D3" s="38"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -3958,12 +4291,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="41"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="45" t="s">
+      <c r="A4" s="42"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="46" t="s">
         <v>230</v>
       </c>
-      <c r="D4" s="37"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -3982,12 +4315,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="43"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="45" t="s">
+      <c r="A5" s="44"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="46" t="s">
         <v>231</v>
       </c>
-      <c r="D5" s="37"/>
+      <c r="D5" s="38"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -4005,8 +4338,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="34"/>
-      <c r="B6" s="35"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -5281,7 +5614,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="24.95" customHeight="1">
+    <row r="32" spans="1:20" ht="24.95" customHeight="1" thickBot="1">
       <c r="A32" s="20">
         <v>372</v>
       </c>
@@ -5327,364 +5660,1103 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
-      <c r="N33" s="13"/>
-      <c r="O33" s="13"/>
-      <c r="P33" s="13"/>
-      <c r="Q33" s="13"/>
-      <c r="R33" s="14"/>
-      <c r="S33" s="2"/>
-      <c r="T33" s="15"/>
-    </row>
-    <row r="34" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="13"/>
-      <c r="M34" s="13"/>
-      <c r="N34" s="13"/>
-      <c r="O34" s="13"/>
-      <c r="P34" s="13"/>
-      <c r="Q34" s="13"/>
-      <c r="R34" s="14"/>
-      <c r="S34" s="2"/>
-      <c r="T34" s="15"/>
-    </row>
-    <row r="35" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="13"/>
-      <c r="O35" s="13"/>
-      <c r="P35" s="13"/>
-      <c r="Q35" s="13"/>
-      <c r="R35" s="14"/>
-      <c r="S35" s="2"/>
-      <c r="T35" s="15"/>
-    </row>
-    <row r="36" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="13"/>
-      <c r="O36" s="13"/>
-      <c r="P36" s="13"/>
-      <c r="Q36" s="13"/>
-      <c r="R36" s="14"/>
-      <c r="S36" s="2"/>
-      <c r="T36" s="15"/>
-    </row>
-    <row r="37" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="13"/>
-      <c r="N37" s="13"/>
-      <c r="O37" s="13"/>
-      <c r="P37" s="13"/>
-      <c r="Q37" s="13"/>
-      <c r="R37" s="14"/>
-      <c r="S37" s="2"/>
-      <c r="T37" s="15"/>
-    </row>
-    <row r="38" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13"/>
-      <c r="L38" s="13"/>
-      <c r="M38" s="13"/>
-      <c r="N38" s="13"/>
-      <c r="O38" s="13"/>
-      <c r="P38" s="13"/>
-      <c r="Q38" s="13"/>
-      <c r="R38" s="14"/>
-      <c r="S38" s="2"/>
-      <c r="T38" s="15"/>
-    </row>
-    <row r="39" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
-      <c r="J39" s="13"/>
-      <c r="K39" s="13"/>
-      <c r="L39" s="13"/>
-      <c r="M39" s="13"/>
-      <c r="N39" s="13"/>
-      <c r="O39" s="13"/>
-      <c r="P39" s="13"/>
-      <c r="Q39" s="13"/>
-      <c r="R39" s="14"/>
-      <c r="S39" s="2"/>
-      <c r="T39" s="15"/>
-    </row>
-    <row r="40" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="12"/>
-      <c r="J40" s="13"/>
-      <c r="K40" s="13"/>
-      <c r="L40" s="13"/>
-      <c r="M40" s="13"/>
-      <c r="N40" s="13"/>
-      <c r="O40" s="13"/>
-      <c r="P40" s="13"/>
-      <c r="Q40" s="13"/>
-      <c r="R40" s="14"/>
-      <c r="S40" s="2"/>
-      <c r="T40" s="15"/>
-    </row>
-    <row r="41" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="13"/>
-      <c r="K41" s="13"/>
-      <c r="L41" s="13"/>
-      <c r="M41" s="13"/>
-      <c r="N41" s="13"/>
-      <c r="O41" s="13"/>
-      <c r="P41" s="13"/>
-      <c r="Q41" s="13"/>
-      <c r="R41" s="14"/>
-      <c r="S41" s="2"/>
-      <c r="T41" s="15"/>
-    </row>
-    <row r="42" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
-      <c r="I42" s="12"/>
-      <c r="J42" s="13"/>
-      <c r="K42" s="13"/>
-      <c r="L42" s="13"/>
-      <c r="M42" s="13"/>
-      <c r="N42" s="13"/>
-      <c r="O42" s="13"/>
-      <c r="P42" s="13"/>
-      <c r="Q42" s="13"/>
-      <c r="R42" s="14"/>
-      <c r="S42" s="2"/>
-      <c r="T42" s="15"/>
-    </row>
-    <row r="43" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
-      <c r="H43" s="12"/>
-      <c r="I43" s="12"/>
-      <c r="J43" s="13"/>
-      <c r="K43" s="13"/>
-      <c r="L43" s="13"/>
-      <c r="M43" s="13"/>
-      <c r="N43" s="13"/>
-      <c r="O43" s="13"/>
-      <c r="P43" s="13"/>
-      <c r="Q43" s="13"/>
-      <c r="R43" s="14"/>
-      <c r="S43" s="2"/>
-      <c r="T43" s="15"/>
-    </row>
-    <row r="44" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="12"/>
-      <c r="J44" s="13"/>
-      <c r="K44" s="13"/>
-      <c r="L44" s="13"/>
-      <c r="M44" s="13"/>
-      <c r="N44" s="13"/>
-      <c r="O44" s="13"/>
-      <c r="P44" s="13"/>
-      <c r="Q44" s="13"/>
-      <c r="R44" s="14"/>
-      <c r="S44" s="2"/>
-      <c r="T44" s="15"/>
-    </row>
-    <row r="45" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="13"/>
-      <c r="K45" s="13"/>
-      <c r="L45" s="13"/>
-      <c r="M45" s="13"/>
-      <c r="N45" s="13"/>
-      <c r="O45" s="13"/>
-      <c r="P45" s="13"/>
-      <c r="Q45" s="13"/>
-      <c r="R45" s="14"/>
-      <c r="S45" s="2"/>
-      <c r="T45" s="15"/>
-    </row>
-    <row r="46" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-      <c r="H46" s="12"/>
-      <c r="I46" s="12"/>
-      <c r="J46" s="13"/>
-      <c r="K46" s="13"/>
-      <c r="L46" s="13"/>
-      <c r="M46" s="13"/>
-      <c r="N46" s="13"/>
-      <c r="O46" s="13"/>
-      <c r="P46" s="13"/>
-      <c r="Q46" s="13"/>
-      <c r="R46" s="14"/>
-      <c r="S46" s="2"/>
-      <c r="T46" s="15"/>
-    </row>
-    <row r="47" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-      <c r="H47" s="12"/>
-      <c r="I47" s="12"/>
-      <c r="J47" s="13"/>
-      <c r="K47" s="13"/>
-      <c r="L47" s="13"/>
-      <c r="M47" s="13"/>
-      <c r="N47" s="13"/>
-      <c r="O47" s="13"/>
-      <c r="P47" s="13"/>
-      <c r="Q47" s="13"/>
-      <c r="R47" s="14"/>
-      <c r="S47" s="2"/>
-      <c r="T47" s="15"/>
-    </row>
-    <row r="48" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-      <c r="H48" s="12"/>
-      <c r="I48" s="12"/>
-      <c r="J48" s="13"/>
-      <c r="K48" s="13"/>
-      <c r="L48" s="13"/>
-      <c r="M48" s="13"/>
-      <c r="N48" s="13"/>
-      <c r="O48" s="13"/>
-      <c r="P48" s="13"/>
-      <c r="Q48" s="13"/>
-      <c r="R48" s="14"/>
-      <c r="S48" s="2"/>
-      <c r="T48" s="15"/>
-    </row>
-    <row r="49" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
-      <c r="H49" s="12"/>
-      <c r="I49" s="12"/>
-      <c r="J49" s="13"/>
-      <c r="K49" s="13"/>
-      <c r="L49" s="13"/>
-      <c r="M49" s="13"/>
-      <c r="N49" s="13"/>
-      <c r="O49" s="13"/>
-      <c r="P49" s="13"/>
-      <c r="Q49" s="13"/>
-      <c r="R49" s="14"/>
-      <c r="S49" s="2"/>
-      <c r="T49" s="15"/>
-    </row>
-    <row r="50" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="12"/>
-      <c r="I50" s="12"/>
-      <c r="J50" s="13"/>
-      <c r="K50" s="13"/>
-      <c r="L50" s="13"/>
-      <c r="M50" s="13"/>
-      <c r="N50" s="13"/>
-      <c r="O50" s="13"/>
-      <c r="P50" s="13"/>
-      <c r="Q50" s="13"/>
-      <c r="R50" s="14"/>
-      <c r="S50" s="2"/>
-      <c r="T50" s="15"/>
-    </row>
-    <row r="51" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
-      <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
-      <c r="J51" s="13"/>
-      <c r="K51" s="13"/>
-      <c r="L51" s="13"/>
-      <c r="M51" s="13"/>
-      <c r="N51" s="13"/>
-      <c r="O51" s="13"/>
-      <c r="P51" s="13"/>
-      <c r="Q51" s="13"/>
-      <c r="R51" s="14"/>
-      <c r="S51" s="2"/>
-      <c r="T51" s="15"/>
-    </row>
-    <row r="52" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F52" s="12"/>
-      <c r="G52" s="12"/>
-      <c r="H52" s="12"/>
-      <c r="I52" s="12"/>
-      <c r="J52" s="13"/>
-      <c r="K52" s="13"/>
-      <c r="L52" s="13"/>
-      <c r="M52" s="13"/>
-      <c r="N52" s="13"/>
-      <c r="O52" s="13"/>
-      <c r="P52" s="13"/>
-      <c r="Q52" s="13"/>
-      <c r="R52" s="14"/>
-      <c r="S52" s="2"/>
-      <c r="T52" s="15"/>
-    </row>
-    <row r="53" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
-      <c r="H53" s="12"/>
-      <c r="I53" s="12"/>
-      <c r="J53" s="13"/>
-      <c r="K53" s="13"/>
-      <c r="L53" s="13"/>
-      <c r="M53" s="13"/>
-      <c r="N53" s="13"/>
-      <c r="O53" s="13"/>
-      <c r="P53" s="13"/>
-      <c r="Q53" s="13"/>
-      <c r="R53" s="14"/>
-      <c r="S53" s="2"/>
-      <c r="T53" s="15"/>
-    </row>
-    <row r="54" spans="6:20" ht="14.25" customHeight="1">
+    <row r="33" spans="1:20" ht="30" customHeight="1" thickBot="1">
+      <c r="A33" s="20">
+        <v>16</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="F33" s="23">
+        <v>45083</v>
+      </c>
+      <c r="G33" s="24" t="s">
+        <v>236</v>
+      </c>
+      <c r="H33" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="I33" s="24" t="s">
+        <v>238</v>
+      </c>
+      <c r="J33" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="K33" s="25"/>
+      <c r="L33" s="25"/>
+      <c r="M33" s="25"/>
+      <c r="N33" s="25"/>
+      <c r="O33" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="P33" s="25"/>
+      <c r="Q33" s="25"/>
+      <c r="R33" s="26"/>
+      <c r="S33" s="27"/>
+      <c r="T33" s="28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" ht="30" customHeight="1" thickBot="1">
+      <c r="A34" s="20">
+        <v>17</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="F34" s="23">
+        <v>45083</v>
+      </c>
+      <c r="G34" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="H34" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="I34" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="J34" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="K34" s="25"/>
+      <c r="L34" s="25"/>
+      <c r="M34" s="25"/>
+      <c r="N34" s="25"/>
+      <c r="O34" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="P34" s="25"/>
+      <c r="Q34" s="25"/>
+      <c r="R34" s="26"/>
+      <c r="S34" s="27"/>
+      <c r="T34" s="28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" ht="30" customHeight="1" thickBot="1">
+      <c r="A35" s="20">
+        <v>18</v>
+      </c>
+      <c r="B35" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="E35" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="F35" s="23">
+        <v>45083</v>
+      </c>
+      <c r="G35" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H35" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="I35" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="J35" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="K35" s="25"/>
+      <c r="L35" s="25"/>
+      <c r="M35" s="25"/>
+      <c r="N35" s="25"/>
+      <c r="O35" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="P35" s="25"/>
+      <c r="Q35" s="25"/>
+      <c r="R35" s="26"/>
+      <c r="S35" s="27"/>
+      <c r="T35" s="28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" ht="30" customHeight="1" thickBot="1">
+      <c r="A36" s="20">
+        <v>19</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="F36" s="23">
+        <v>45083</v>
+      </c>
+      <c r="G36" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="H36" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="I36" s="24" t="s">
+        <v>253</v>
+      </c>
+      <c r="J36" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="K36" s="25"/>
+      <c r="L36" s="25"/>
+      <c r="M36" s="25"/>
+      <c r="N36" s="25"/>
+      <c r="O36" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="P36" s="25"/>
+      <c r="Q36" s="25"/>
+      <c r="R36" s="26"/>
+      <c r="S36" s="27"/>
+      <c r="T36" s="28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" ht="30" customHeight="1" thickBot="1">
+      <c r="A37" s="20">
+        <v>33</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>254</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="F37" s="23">
+        <v>45083</v>
+      </c>
+      <c r="G37" s="24" t="s">
+        <v>255</v>
+      </c>
+      <c r="H37" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="I37" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="J37" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="K37" s="25"/>
+      <c r="L37" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="M37" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="N37" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="O37" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="P37" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q37" s="25"/>
+      <c r="R37" s="26"/>
+      <c r="S37" s="27"/>
+      <c r="T37" s="28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" ht="30" customHeight="1" thickBot="1">
+      <c r="A38" s="20">
+        <v>41</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>257</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="F38" s="23">
+        <v>45083</v>
+      </c>
+      <c r="G38" s="24" t="s">
+        <v>258</v>
+      </c>
+      <c r="H38" s="24" t="s">
+        <v>259</v>
+      </c>
+      <c r="I38" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="J38" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="K38" s="25"/>
+      <c r="L38" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="M38" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="N38" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="O38" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="P38" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q38" s="25"/>
+      <c r="R38" s="26"/>
+      <c r="S38" s="27"/>
+      <c r="T38" s="28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" ht="30" customHeight="1" thickBot="1">
+      <c r="A39" s="20">
+        <v>49</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="F39" s="23">
+        <v>45083</v>
+      </c>
+      <c r="G39" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="H39" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="I39" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="J39" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="K39" s="25"/>
+      <c r="L39" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="M39" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="N39" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="O39" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="P39" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q39" s="25"/>
+      <c r="R39" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="S39" s="27"/>
+      <c r="T39" s="28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" ht="30" customHeight="1" thickBot="1">
+      <c r="A40" s="20">
+        <v>94</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D40" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="E40" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="F40" s="23">
+        <v>45083</v>
+      </c>
+      <c r="G40" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="H40" s="24" t="s">
+        <v>264</v>
+      </c>
+      <c r="I40" s="24" t="s">
+        <v>265</v>
+      </c>
+      <c r="J40" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="K40" s="25"/>
+      <c r="L40" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="M40" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="N40" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="O40" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="P40" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q40" s="25"/>
+      <c r="R40" s="26"/>
+      <c r="S40" s="27"/>
+      <c r="T40" s="28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" ht="30" customHeight="1" thickBot="1">
+      <c r="A41" s="20">
+        <v>95</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="E41" s="22" t="s">
+        <v>267</v>
+      </c>
+      <c r="F41" s="23">
+        <v>45083</v>
+      </c>
+      <c r="G41" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="H41" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="I41" s="24" t="s">
+        <v>270</v>
+      </c>
+      <c r="J41" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="K41" s="25"/>
+      <c r="L41" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="M41" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="N41" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="O41" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="P41" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q41" s="25"/>
+      <c r="R41" s="26"/>
+      <c r="S41" s="27"/>
+      <c r="T41" s="28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" ht="30" customHeight="1" thickBot="1">
+      <c r="A42" s="20">
+        <v>96</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>271</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>272</v>
+      </c>
+      <c r="F42" s="23">
+        <v>45083</v>
+      </c>
+      <c r="G42" s="24" t="s">
+        <v>273</v>
+      </c>
+      <c r="H42" s="24" t="s">
+        <v>274</v>
+      </c>
+      <c r="I42" s="24" t="s">
+        <v>275</v>
+      </c>
+      <c r="J42" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="K42" s="25"/>
+      <c r="L42" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="M42" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="N42" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="O42" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="P42" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q42" s="25"/>
+      <c r="R42" s="26"/>
+      <c r="S42" s="27"/>
+      <c r="T42" s="28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" ht="30" customHeight="1" thickBot="1">
+      <c r="A43" s="20">
+        <v>97</v>
+      </c>
+      <c r="B43" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D43" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="E43" s="22" t="s">
+        <v>277</v>
+      </c>
+      <c r="F43" s="23">
+        <v>45083</v>
+      </c>
+      <c r="G43" s="24" t="s">
+        <v>278</v>
+      </c>
+      <c r="H43" s="24" t="s">
+        <v>279</v>
+      </c>
+      <c r="I43" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="J43" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="K43" s="25"/>
+      <c r="L43" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="M43" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="N43" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="O43" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="P43" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q43" s="25"/>
+      <c r="R43" s="26"/>
+      <c r="S43" s="27"/>
+      <c r="T43" s="28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" ht="30" customHeight="1" thickBot="1">
+      <c r="A44" s="20">
+        <v>98</v>
+      </c>
+      <c r="B44" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>281</v>
+      </c>
+      <c r="E44" s="22" t="s">
+        <v>282</v>
+      </c>
+      <c r="F44" s="23">
+        <v>45083</v>
+      </c>
+      <c r="G44" s="24" t="s">
+        <v>283</v>
+      </c>
+      <c r="H44" s="24" t="s">
+        <v>284</v>
+      </c>
+      <c r="I44" s="24" t="s">
+        <v>285</v>
+      </c>
+      <c r="J44" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="K44" s="25"/>
+      <c r="L44" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="M44" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="N44" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="O44" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="P44" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q44" s="25"/>
+      <c r="R44" s="26"/>
+      <c r="S44" s="27"/>
+      <c r="T44" s="28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" ht="30" customHeight="1" thickBot="1">
+      <c r="A45" s="20">
+        <v>99</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>286</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>287</v>
+      </c>
+      <c r="F45" s="23">
+        <v>45083</v>
+      </c>
+      <c r="G45" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="H45" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="I45" s="24" t="s">
+        <v>290</v>
+      </c>
+      <c r="J45" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="K45" s="25"/>
+      <c r="L45" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="M45" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="N45" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="O45" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="P45" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q45" s="25"/>
+      <c r="R45" s="26"/>
+      <c r="S45" s="27"/>
+      <c r="T45" s="28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" ht="30" customHeight="1" thickBot="1">
+      <c r="A46" s="20">
+        <v>100</v>
+      </c>
+      <c r="B46" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>292</v>
+      </c>
+      <c r="F46" s="23">
+        <v>45083</v>
+      </c>
+      <c r="G46" s="24" t="s">
+        <v>293</v>
+      </c>
+      <c r="H46" s="24" t="s">
+        <v>294</v>
+      </c>
+      <c r="I46" s="24" t="s">
+        <v>295</v>
+      </c>
+      <c r="J46" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="K46" s="25"/>
+      <c r="L46" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="M46" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="N46" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="O46" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="P46" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q46" s="25"/>
+      <c r="R46" s="26"/>
+      <c r="S46" s="27"/>
+      <c r="T46" s="28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" ht="30" customHeight="1" thickBot="1">
+      <c r="A47" s="20">
+        <v>101</v>
+      </c>
+      <c r="B47" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" s="21" t="s">
+        <v>296</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>297</v>
+      </c>
+      <c r="F47" s="23">
+        <v>45083</v>
+      </c>
+      <c r="G47" s="24" t="s">
+        <v>298</v>
+      </c>
+      <c r="H47" s="24" t="s">
+        <v>299</v>
+      </c>
+      <c r="I47" s="24" t="s">
+        <v>300</v>
+      </c>
+      <c r="J47" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="K47" s="25"/>
+      <c r="L47" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="M47" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="N47" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="O47" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="P47" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q47" s="25"/>
+      <c r="R47" s="26"/>
+      <c r="S47" s="27"/>
+      <c r="T47" s="28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" ht="30" customHeight="1" thickBot="1">
+      <c r="A48" s="20">
+        <v>102</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D48" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>302</v>
+      </c>
+      <c r="F48" s="23">
+        <v>45083</v>
+      </c>
+      <c r="G48" s="24" t="s">
+        <v>303</v>
+      </c>
+      <c r="H48" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="I48" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="J48" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="K48" s="25"/>
+      <c r="L48" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="M48" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="N48" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="O48" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="P48" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q48" s="25"/>
+      <c r="R48" s="26"/>
+      <c r="S48" s="27"/>
+      <c r="T48" s="28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" ht="30" customHeight="1" thickBot="1">
+      <c r="A49" s="20">
+        <v>103</v>
+      </c>
+      <c r="B49" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C49" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>306</v>
+      </c>
+      <c r="E49" s="22" t="s">
+        <v>307</v>
+      </c>
+      <c r="F49" s="23">
+        <v>45083</v>
+      </c>
+      <c r="G49" s="24" t="s">
+        <v>308</v>
+      </c>
+      <c r="H49" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="I49" s="24" t="s">
+        <v>310</v>
+      </c>
+      <c r="J49" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="K49" s="25"/>
+      <c r="L49" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="M49" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="N49" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="O49" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="P49" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q49" s="25"/>
+      <c r="R49" s="26"/>
+      <c r="S49" s="27"/>
+      <c r="T49" s="28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" ht="30" customHeight="1" thickBot="1">
+      <c r="A50" s="20">
+        <v>104</v>
+      </c>
+      <c r="B50" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C50" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>311</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>312</v>
+      </c>
+      <c r="F50" s="23">
+        <v>45083</v>
+      </c>
+      <c r="G50" s="24" t="s">
+        <v>313</v>
+      </c>
+      <c r="H50" s="24" t="s">
+        <v>314</v>
+      </c>
+      <c r="I50" s="24" t="s">
+        <v>315</v>
+      </c>
+      <c r="J50" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="K50" s="25"/>
+      <c r="L50" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="M50" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="N50" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="O50" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="P50" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q50" s="25"/>
+      <c r="R50" s="26"/>
+      <c r="S50" s="27"/>
+      <c r="T50" s="28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" ht="30" customHeight="1" thickBot="1">
+      <c r="A51" s="20">
+        <v>105</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D51" s="21" t="s">
+        <v>316</v>
+      </c>
+      <c r="E51" s="22" t="s">
+        <v>317</v>
+      </c>
+      <c r="F51" s="23">
+        <v>45083</v>
+      </c>
+      <c r="G51" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="H51" s="24" t="s">
+        <v>319</v>
+      </c>
+      <c r="I51" s="24" t="s">
+        <v>320</v>
+      </c>
+      <c r="J51" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="K51" s="25"/>
+      <c r="L51" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="M51" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="N51" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="O51" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="P51" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q51" s="25"/>
+      <c r="R51" s="26"/>
+      <c r="S51" s="27"/>
+      <c r="T51" s="28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" ht="30" customHeight="1" thickBot="1">
+      <c r="A52" s="20">
+        <v>106</v>
+      </c>
+      <c r="B52" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C52" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D52" s="21" t="s">
+        <v>321</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>322</v>
+      </c>
+      <c r="F52" s="23">
+        <v>45083</v>
+      </c>
+      <c r="G52" s="24" t="s">
+        <v>323</v>
+      </c>
+      <c r="H52" s="24" t="s">
+        <v>324</v>
+      </c>
+      <c r="I52" s="24" t="s">
+        <v>325</v>
+      </c>
+      <c r="J52" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="K52" s="25"/>
+      <c r="L52" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="M52" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="N52" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="O52" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="P52" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q52" s="25"/>
+      <c r="R52" s="26"/>
+      <c r="S52" s="27"/>
+      <c r="T52" s="28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" ht="30" customHeight="1">
+      <c r="A53" s="20">
+        <v>371</v>
+      </c>
+      <c r="B53" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C53" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D53" s="21" t="s">
+        <v>326</v>
+      </c>
+      <c r="E53" s="22" t="s">
+        <v>327</v>
+      </c>
+      <c r="F53" s="23">
+        <v>45092</v>
+      </c>
+      <c r="G53" s="24" t="s">
+        <v>328</v>
+      </c>
+      <c r="H53" s="34" t="s">
+        <v>329</v>
+      </c>
+      <c r="I53" s="24" t="s">
+        <v>330</v>
+      </c>
+      <c r="J53" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="K53" s="25"/>
+      <c r="L53" s="25"/>
+      <c r="M53" s="25"/>
+      <c r="N53" s="33"/>
+      <c r="O53" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="P53" s="33"/>
+      <c r="Q53" s="25"/>
+      <c r="R53" s="26"/>
+      <c r="S53" s="27"/>
+      <c r="T53" s="28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" ht="14.25" customHeight="1">
       <c r="F54" s="12"/>
       <c r="G54" s="12"/>
       <c r="H54" s="12"/>
@@ -5701,7 +6773,7 @@
       <c r="S54" s="2"/>
       <c r="T54" s="15"/>
     </row>
-    <row r="55" spans="6:20" ht="14.25" customHeight="1">
+    <row r="55" spans="1:20" ht="14.25" customHeight="1">
       <c r="F55" s="12"/>
       <c r="G55" s="12"/>
       <c r="H55" s="12"/>
@@ -5718,7 +6790,7 @@
       <c r="S55" s="2"/>
       <c r="T55" s="15"/>
     </row>
-    <row r="56" spans="6:20" ht="14.25" customHeight="1">
+    <row r="56" spans="1:20" ht="14.25" customHeight="1">
       <c r="F56" s="12"/>
       <c r="G56" s="12"/>
       <c r="H56" s="12"/>
@@ -5735,7 +6807,7 @@
       <c r="S56" s="2"/>
       <c r="T56" s="15"/>
     </row>
-    <row r="57" spans="6:20" ht="14.25" customHeight="1">
+    <row r="57" spans="1:20" ht="14.25" customHeight="1">
       <c r="F57" s="12"/>
       <c r="G57" s="12"/>
       <c r="H57" s="12"/>
@@ -5752,7 +6824,7 @@
       <c r="S57" s="2"/>
       <c r="T57" s="15"/>
     </row>
-    <row r="58" spans="6:20" ht="14.25" customHeight="1">
+    <row r="58" spans="1:20" ht="14.25" customHeight="1">
       <c r="F58" s="12"/>
       <c r="G58" s="12"/>
       <c r="H58" s="12"/>
@@ -5769,7 +6841,7 @@
       <c r="S58" s="2"/>
       <c r="T58" s="15"/>
     </row>
-    <row r="59" spans="6:20" ht="14.25" customHeight="1">
+    <row r="59" spans="1:20" ht="14.25" customHeight="1">
       <c r="F59" s="12"/>
       <c r="G59" s="12"/>
       <c r="H59" s="12"/>
@@ -5786,7 +6858,7 @@
       <c r="S59" s="2"/>
       <c r="T59" s="15"/>
     </row>
-    <row r="60" spans="6:20" ht="14.25" customHeight="1">
+    <row r="60" spans="1:20" ht="14.25" customHeight="1">
       <c r="F60" s="12"/>
       <c r="G60" s="12"/>
       <c r="H60" s="12"/>
@@ -5803,7 +6875,7 @@
       <c r="S60" s="2"/>
       <c r="T60" s="15"/>
     </row>
-    <row r="61" spans="6:20" ht="14.25" customHeight="1">
+    <row r="61" spans="1:20" ht="14.25" customHeight="1">
       <c r="F61" s="12"/>
       <c r="G61" s="12"/>
       <c r="H61" s="12"/>
@@ -5820,7 +6892,7 @@
       <c r="S61" s="2"/>
       <c r="T61" s="15"/>
     </row>
-    <row r="62" spans="6:20" ht="14.25" customHeight="1">
+    <row r="62" spans="1:20" ht="14.25" customHeight="1">
       <c r="F62" s="12"/>
       <c r="G62" s="12"/>
       <c r="H62" s="12"/>
@@ -5837,7 +6909,7 @@
       <c r="S62" s="2"/>
       <c r="T62" s="15"/>
     </row>
-    <row r="63" spans="6:20" ht="14.25" customHeight="1">
+    <row r="63" spans="1:20" ht="14.25" customHeight="1">
       <c r="F63" s="12"/>
       <c r="G63" s="12"/>
       <c r="H63" s="12"/>
@@ -5854,7 +6926,7 @@
       <c r="S63" s="2"/>
       <c r="T63" s="15"/>
     </row>
-    <row r="64" spans="6:20" ht="14.25" customHeight="1">
+    <row r="64" spans="1:20" ht="14.25" customHeight="1">
       <c r="F64" s="12"/>
       <c r="G64" s="12"/>
       <c r="H64" s="12"/>
@@ -8388,367 +9460,87 @@
       <c r="T212" s="15"/>
     </row>
     <row r="213" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F213" s="12"/>
-      <c r="G213" s="12"/>
-      <c r="H213" s="12"/>
-      <c r="I213" s="12"/>
-      <c r="J213" s="13"/>
-      <c r="K213" s="13"/>
-      <c r="L213" s="13"/>
-      <c r="M213" s="13"/>
-      <c r="N213" s="13"/>
-      <c r="O213" s="13"/>
-      <c r="P213" s="13"/>
-      <c r="Q213" s="13"/>
-      <c r="R213" s="14"/>
-      <c r="S213" s="2"/>
-      <c r="T213" s="15"/>
+      <c r="T213" s="13"/>
     </row>
     <row r="214" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F214" s="12"/>
-      <c r="G214" s="12"/>
-      <c r="H214" s="12"/>
-      <c r="I214" s="12"/>
-      <c r="J214" s="13"/>
-      <c r="K214" s="13"/>
-      <c r="L214" s="13"/>
-      <c r="M214" s="13"/>
-      <c r="N214" s="13"/>
-      <c r="O214" s="13"/>
-      <c r="P214" s="13"/>
-      <c r="Q214" s="13"/>
-      <c r="R214" s="14"/>
-      <c r="S214" s="2"/>
-      <c r="T214" s="15"/>
+      <c r="T214" s="13"/>
     </row>
     <row r="215" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F215" s="12"/>
-      <c r="G215" s="12"/>
-      <c r="H215" s="12"/>
-      <c r="I215" s="12"/>
-      <c r="J215" s="13"/>
-      <c r="K215" s="13"/>
-      <c r="L215" s="13"/>
-      <c r="M215" s="13"/>
-      <c r="N215" s="13"/>
-      <c r="O215" s="13"/>
-      <c r="P215" s="13"/>
-      <c r="Q215" s="13"/>
-      <c r="R215" s="14"/>
-      <c r="S215" s="2"/>
-      <c r="T215" s="15"/>
+      <c r="T215" s="13"/>
     </row>
     <row r="216" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F216" s="12"/>
-      <c r="G216" s="12"/>
-      <c r="H216" s="12"/>
-      <c r="I216" s="12"/>
-      <c r="J216" s="13"/>
-      <c r="K216" s="13"/>
-      <c r="L216" s="13"/>
-      <c r="M216" s="13"/>
-      <c r="N216" s="13"/>
-      <c r="O216" s="13"/>
-      <c r="P216" s="13"/>
-      <c r="Q216" s="13"/>
-      <c r="R216" s="14"/>
-      <c r="S216" s="2"/>
-      <c r="T216" s="15"/>
+      <c r="T216" s="13"/>
     </row>
     <row r="217" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F217" s="12"/>
-      <c r="G217" s="12"/>
-      <c r="H217" s="12"/>
-      <c r="I217" s="12"/>
-      <c r="J217" s="13"/>
-      <c r="K217" s="13"/>
-      <c r="L217" s="13"/>
-      <c r="M217" s="13"/>
-      <c r="N217" s="13"/>
-      <c r="O217" s="13"/>
-      <c r="P217" s="13"/>
-      <c r="Q217" s="13"/>
-      <c r="R217" s="14"/>
-      <c r="S217" s="2"/>
-      <c r="T217" s="15"/>
+      <c r="T217" s="13"/>
     </row>
     <row r="218" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F218" s="12"/>
-      <c r="G218" s="12"/>
-      <c r="H218" s="12"/>
-      <c r="I218" s="12"/>
-      <c r="J218" s="13"/>
-      <c r="K218" s="13"/>
-      <c r="L218" s="13"/>
-      <c r="M218" s="13"/>
-      <c r="N218" s="13"/>
-      <c r="O218" s="13"/>
-      <c r="P218" s="13"/>
-      <c r="Q218" s="13"/>
-      <c r="R218" s="14"/>
-      <c r="S218" s="2"/>
-      <c r="T218" s="15"/>
+      <c r="T218" s="13"/>
     </row>
     <row r="219" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F219" s="12"/>
-      <c r="G219" s="12"/>
-      <c r="H219" s="12"/>
-      <c r="I219" s="12"/>
-      <c r="J219" s="13"/>
-      <c r="K219" s="13"/>
-      <c r="L219" s="13"/>
-      <c r="M219" s="13"/>
-      <c r="N219" s="13"/>
-      <c r="O219" s="13"/>
-      <c r="P219" s="13"/>
-      <c r="Q219" s="13"/>
-      <c r="R219" s="14"/>
-      <c r="S219" s="2"/>
-      <c r="T219" s="15"/>
+      <c r="T219" s="13"/>
     </row>
     <row r="220" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F220" s="12"/>
-      <c r="G220" s="12"/>
-      <c r="H220" s="12"/>
-      <c r="I220" s="12"/>
-      <c r="J220" s="13"/>
-      <c r="K220" s="13"/>
-      <c r="L220" s="13"/>
-      <c r="M220" s="13"/>
-      <c r="N220" s="13"/>
-      <c r="O220" s="13"/>
-      <c r="P220" s="13"/>
-      <c r="Q220" s="13"/>
-      <c r="R220" s="14"/>
-      <c r="S220" s="2"/>
-      <c r="T220" s="15"/>
+      <c r="T220" s="13"/>
     </row>
     <row r="221" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F221" s="12"/>
-      <c r="G221" s="12"/>
-      <c r="H221" s="12"/>
-      <c r="I221" s="12"/>
-      <c r="J221" s="13"/>
-      <c r="K221" s="13"/>
-      <c r="L221" s="13"/>
-      <c r="M221" s="13"/>
-      <c r="N221" s="13"/>
-      <c r="O221" s="13"/>
-      <c r="P221" s="13"/>
-      <c r="Q221" s="13"/>
-      <c r="R221" s="14"/>
-      <c r="S221" s="2"/>
-      <c r="T221" s="15"/>
+      <c r="T221" s="13"/>
     </row>
     <row r="222" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F222" s="12"/>
-      <c r="G222" s="12"/>
-      <c r="H222" s="12"/>
-      <c r="I222" s="12"/>
-      <c r="J222" s="13"/>
-      <c r="K222" s="13"/>
-      <c r="L222" s="13"/>
-      <c r="M222" s="13"/>
-      <c r="N222" s="13"/>
-      <c r="O222" s="13"/>
-      <c r="P222" s="13"/>
-      <c r="Q222" s="13"/>
-      <c r="R222" s="14"/>
-      <c r="S222" s="2"/>
-      <c r="T222" s="15"/>
+      <c r="T222" s="13"/>
     </row>
     <row r="223" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F223" s="12"/>
-      <c r="G223" s="12"/>
-      <c r="H223" s="12"/>
-      <c r="I223" s="12"/>
-      <c r="J223" s="13"/>
-      <c r="K223" s="13"/>
-      <c r="L223" s="13"/>
-      <c r="M223" s="13"/>
-      <c r="N223" s="13"/>
-      <c r="O223" s="13"/>
-      <c r="P223" s="13"/>
-      <c r="Q223" s="13"/>
-      <c r="R223" s="14"/>
-      <c r="S223" s="2"/>
-      <c r="T223" s="15"/>
+      <c r="T223" s="13"/>
     </row>
     <row r="224" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F224" s="12"/>
-      <c r="G224" s="12"/>
-      <c r="H224" s="12"/>
-      <c r="I224" s="12"/>
-      <c r="J224" s="13"/>
-      <c r="K224" s="13"/>
-      <c r="L224" s="13"/>
-      <c r="M224" s="13"/>
-      <c r="N224" s="13"/>
-      <c r="O224" s="13"/>
-      <c r="P224" s="13"/>
-      <c r="Q224" s="13"/>
-      <c r="R224" s="14"/>
-      <c r="S224" s="2"/>
-      <c r="T224" s="15"/>
-    </row>
-    <row r="225" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F225" s="12"/>
-      <c r="G225" s="12"/>
-      <c r="H225" s="12"/>
-      <c r="I225" s="12"/>
-      <c r="J225" s="13"/>
-      <c r="K225" s="13"/>
-      <c r="L225" s="13"/>
-      <c r="M225" s="13"/>
-      <c r="N225" s="13"/>
-      <c r="O225" s="13"/>
-      <c r="P225" s="13"/>
-      <c r="Q225" s="13"/>
-      <c r="R225" s="14"/>
-      <c r="S225" s="2"/>
-      <c r="T225" s="15"/>
-    </row>
-    <row r="226" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F226" s="12"/>
-      <c r="G226" s="12"/>
-      <c r="H226" s="12"/>
-      <c r="I226" s="12"/>
-      <c r="J226" s="13"/>
-      <c r="K226" s="13"/>
-      <c r="L226" s="13"/>
-      <c r="M226" s="13"/>
-      <c r="N226" s="13"/>
-      <c r="O226" s="13"/>
-      <c r="P226" s="13"/>
-      <c r="Q226" s="13"/>
-      <c r="R226" s="14"/>
-      <c r="S226" s="2"/>
-      <c r="T226" s="15"/>
-    </row>
-    <row r="227" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F227" s="12"/>
-      <c r="G227" s="12"/>
-      <c r="H227" s="12"/>
-      <c r="I227" s="12"/>
-      <c r="J227" s="13"/>
-      <c r="K227" s="13"/>
-      <c r="L227" s="13"/>
-      <c r="M227" s="13"/>
-      <c r="N227" s="13"/>
-      <c r="O227" s="13"/>
-      <c r="P227" s="13"/>
-      <c r="Q227" s="13"/>
-      <c r="R227" s="14"/>
-      <c r="S227" s="2"/>
-      <c r="T227" s="15"/>
-    </row>
-    <row r="228" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F228" s="12"/>
-      <c r="G228" s="12"/>
-      <c r="H228" s="12"/>
-      <c r="I228" s="12"/>
-      <c r="J228" s="13"/>
-      <c r="K228" s="13"/>
-      <c r="L228" s="13"/>
-      <c r="M228" s="13"/>
-      <c r="N228" s="13"/>
-      <c r="O228" s="13"/>
-      <c r="P228" s="13"/>
-      <c r="Q228" s="13"/>
-      <c r="R228" s="14"/>
-      <c r="S228" s="2"/>
-      <c r="T228" s="15"/>
-    </row>
-    <row r="229" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F229" s="12"/>
-      <c r="G229" s="12"/>
-      <c r="H229" s="12"/>
-      <c r="I229" s="12"/>
-      <c r="J229" s="13"/>
-      <c r="K229" s="13"/>
-      <c r="L229" s="13"/>
-      <c r="M229" s="13"/>
-      <c r="N229" s="13"/>
-      <c r="O229" s="13"/>
-      <c r="P229" s="13"/>
-      <c r="Q229" s="13"/>
-      <c r="R229" s="14"/>
-      <c r="S229" s="2"/>
-      <c r="T229" s="15"/>
-    </row>
-    <row r="230" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F230" s="12"/>
-      <c r="G230" s="12"/>
-      <c r="H230" s="12"/>
-      <c r="I230" s="12"/>
-      <c r="J230" s="13"/>
-      <c r="K230" s="13"/>
-      <c r="L230" s="13"/>
-      <c r="M230" s="13"/>
-      <c r="N230" s="13"/>
-      <c r="O230" s="13"/>
-      <c r="P230" s="13"/>
-      <c r="Q230" s="13"/>
-      <c r="R230" s="14"/>
-      <c r="S230" s="2"/>
-      <c r="T230" s="15"/>
-    </row>
-    <row r="231" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F231" s="12"/>
-      <c r="G231" s="12"/>
-      <c r="H231" s="12"/>
-      <c r="I231" s="12"/>
-      <c r="J231" s="13"/>
-      <c r="K231" s="13"/>
-      <c r="L231" s="13"/>
-      <c r="M231" s="13"/>
-      <c r="N231" s="13"/>
-      <c r="O231" s="13"/>
-      <c r="P231" s="13"/>
-      <c r="Q231" s="13"/>
-      <c r="R231" s="14"/>
-      <c r="S231" s="2"/>
-      <c r="T231" s="15"/>
-    </row>
-    <row r="232" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F232" s="12"/>
-      <c r="G232" s="12"/>
-      <c r="H232" s="12"/>
-      <c r="I232" s="12"/>
-      <c r="J232" s="13"/>
-      <c r="K232" s="13"/>
-      <c r="L232" s="13"/>
-      <c r="M232" s="13"/>
-      <c r="N232" s="13"/>
-      <c r="O232" s="13"/>
-      <c r="P232" s="13"/>
-      <c r="Q232" s="13"/>
-      <c r="R232" s="14"/>
-      <c r="S232" s="2"/>
-      <c r="T232" s="15"/>
-    </row>
-    <row r="233" spans="6:20" ht="14.25" customHeight="1">
+      <c r="T224" s="13"/>
+    </row>
+    <row r="225" spans="20:20" ht="14.25" customHeight="1">
+      <c r="T225" s="13"/>
+    </row>
+    <row r="226" spans="20:20" ht="14.25" customHeight="1">
+      <c r="T226" s="13"/>
+    </row>
+    <row r="227" spans="20:20" ht="14.25" customHeight="1">
+      <c r="T227" s="13"/>
+    </row>
+    <row r="228" spans="20:20" ht="14.25" customHeight="1">
+      <c r="T228" s="13"/>
+    </row>
+    <row r="229" spans="20:20" ht="14.25" customHeight="1">
+      <c r="T229" s="13"/>
+    </row>
+    <row r="230" spans="20:20" ht="14.25" customHeight="1">
+      <c r="T230" s="13"/>
+    </row>
+    <row r="231" spans="20:20" ht="14.25" customHeight="1">
+      <c r="T231" s="13"/>
+    </row>
+    <row r="232" spans="20:20" ht="14.25" customHeight="1">
+      <c r="T232" s="13"/>
+    </row>
+    <row r="233" spans="20:20" ht="14.25" customHeight="1">
       <c r="T233" s="13"/>
     </row>
-    <row r="234" spans="6:20" ht="14.25" customHeight="1">
+    <row r="234" spans="20:20" ht="14.25" customHeight="1">
       <c r="T234" s="13"/>
     </row>
-    <row r="235" spans="6:20" ht="14.25" customHeight="1">
+    <row r="235" spans="20:20" ht="14.25" customHeight="1">
       <c r="T235" s="13"/>
     </row>
-    <row r="236" spans="6:20" ht="14.25" customHeight="1">
+    <row r="236" spans="20:20" ht="14.25" customHeight="1">
       <c r="T236" s="13"/>
     </row>
-    <row r="237" spans="6:20" ht="14.25" customHeight="1">
+    <row r="237" spans="20:20" ht="14.25" customHeight="1">
       <c r="T237" s="13"/>
     </row>
-    <row r="238" spans="6:20" ht="14.25" customHeight="1">
+    <row r="238" spans="20:20" ht="14.25" customHeight="1">
       <c r="T238" s="13"/>
     </row>
-    <row r="239" spans="6:20" ht="14.25" customHeight="1">
+    <row r="239" spans="20:20" ht="14.25" customHeight="1">
       <c r="T239" s="13"/>
     </row>
-    <row r="240" spans="6:20" ht="14.25" customHeight="1">
+    <row r="240" spans="20:20" ht="14.25" customHeight="1">
       <c r="T240" s="13"/>
     </row>
     <row r="241" spans="20:20" ht="14.25" customHeight="1">
@@ -9917,66 +10709,6 @@
     </row>
     <row r="629" spans="20:20" ht="14.25" customHeight="1">
       <c r="T629" s="13"/>
-    </row>
-    <row r="630" spans="20:20" ht="14.25" customHeight="1">
-      <c r="T630" s="13"/>
-    </row>
-    <row r="631" spans="20:20" ht="14.25" customHeight="1">
-      <c r="T631" s="13"/>
-    </row>
-    <row r="632" spans="20:20" ht="14.25" customHeight="1">
-      <c r="T632" s="13"/>
-    </row>
-    <row r="633" spans="20:20" ht="14.25" customHeight="1">
-      <c r="T633" s="13"/>
-    </row>
-    <row r="634" spans="20:20" ht="14.25" customHeight="1">
-      <c r="T634" s="13"/>
-    </row>
-    <row r="635" spans="20:20" ht="14.25" customHeight="1">
-      <c r="T635" s="13"/>
-    </row>
-    <row r="636" spans="20:20" ht="14.25" customHeight="1">
-      <c r="T636" s="13"/>
-    </row>
-    <row r="637" spans="20:20" ht="14.25" customHeight="1">
-      <c r="T637" s="13"/>
-    </row>
-    <row r="638" spans="20:20" ht="14.25" customHeight="1">
-      <c r="T638" s="13"/>
-    </row>
-    <row r="639" spans="20:20" ht="14.25" customHeight="1">
-      <c r="T639" s="13"/>
-    </row>
-    <row r="640" spans="20:20" ht="14.25" customHeight="1">
-      <c r="T640" s="13"/>
-    </row>
-    <row r="641" spans="20:20" ht="14.25" customHeight="1">
-      <c r="T641" s="13"/>
-    </row>
-    <row r="642" spans="20:20" ht="14.25" customHeight="1">
-      <c r="T642" s="13"/>
-    </row>
-    <row r="643" spans="20:20" ht="14.25" customHeight="1">
-      <c r="T643" s="13"/>
-    </row>
-    <row r="644" spans="20:20" ht="14.25" customHeight="1">
-      <c r="T644" s="13"/>
-    </row>
-    <row r="645" spans="20:20" ht="14.25" customHeight="1">
-      <c r="T645" s="13"/>
-    </row>
-    <row r="646" spans="20:20" ht="14.25" customHeight="1">
-      <c r="T646" s="13"/>
-    </row>
-    <row r="647" spans="20:20" ht="14.25" customHeight="1">
-      <c r="T647" s="13"/>
-    </row>
-    <row r="648" spans="20:20" ht="14.25" customHeight="1">
-      <c r="T648" s="13"/>
-    </row>
-    <row r="649" spans="20:20" ht="14.25" customHeight="1">
-      <c r="T649" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A9:T32" xr:uid="{00000000-0009-0000-0000-000002000000}">

</xml_diff>

<commit_message>
Correzione TS test precedenti
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111TOPGATEXXXX/topgate/skipper/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111TOPGATEXXXX/topgate/skipper/1.0/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elia\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F7FC6F-F3EF-4FB6-997B-B4B52F7C00A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E8B915-0E42-46B0-9728-27D1B204A8F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -983,15 +983,6 @@
 Il Documento CDA2 Certificato Vaccinale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-06-06T14:06:10+00:00</t>
-  </si>
-  <si>
-    <t>40c6d620c01ab39a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.9bf750de30^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_CERT_VAC_CT2</t>
   </si>
   <si>
@@ -1000,15 +991,6 @@
 Il Documento CDA2 Certificato Vaccinale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-06-06T14:06:59+00:00</t>
-  </si>
-  <si>
-    <t>066665575e7d6464</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.31d006c495^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_CERT_VAC_CT3</t>
   </si>
   <si>
@@ -1017,15 +999,6 @@
 Il Documento CDA2 Certificato Vaccinale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-06-06T14:07:29+00:00</t>
-  </si>
-  <si>
-    <t>2c460b1311a71f7a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.5868207c1b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_CERT_VAC_CT4</t>
   </si>
   <si>
@@ -1034,31 +1007,10 @@
 Il Documento CDA2 Certificato Vaccinale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-06-06T14:08:03+00:00</t>
-  </si>
-  <si>
-    <t>47ac2f953953c692</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.2db33999b6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_TOKEN_JWT_CERT_VAC_KO</t>
   </si>
   <si>
-    <t>2023-06-06T14:22:02+00:00</t>
-  </si>
-  <si>
-    <t>689f600b08ad0fa9</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_CERT_VAC_KO</t>
-  </si>
-  <si>
-    <t>2023-06-06T14:24:15+00:00</t>
-  </si>
-  <si>
-    <t>8a6db0fc31f11786</t>
   </si>
   <si>
     <t>VALIDAZIONE_CERT_VAC_TIMEOUT</t>
@@ -1072,15 +1024,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-06-06T14:26:36+00:00</t>
-  </si>
-  <si>
-    <t>5615f038ea95218c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.75c7ba1cde^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_CERT_VAC_CT6_KO</t>
   </si>
   <si>
@@ -1089,29 +1032,11 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-06-06T14:29:00+00:00</t>
-  </si>
-  <si>
-    <t>3fd1e4a3162608f8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.337387c473^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_CERT_VAC_CT7_KO</t>
   </si>
   <si>
     <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>2023-06-06T14:30:39+00:00</t>
-  </si>
-  <si>
-    <t>df90246cc8583e8a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.f92e843f53^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_CERT_VAC_CT8_KO</t>
@@ -1122,15 +1047,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-06-06T14:31:19+00:00</t>
-  </si>
-  <si>
-    <t>7ca2d24a0fcd0dc1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.d145185cae^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_CERT_VAC_CT9_KO</t>
   </si>
   <si>
@@ -1139,15 +1055,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-06-06T14:31:45+00:00</t>
-  </si>
-  <si>
-    <t>ddcce3fd35ea2ede</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.feb15d4b48^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_CERT_VAC_CT10_KO</t>
   </si>
   <si>
@@ -1156,29 +1063,11 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-06-06T14:32:21+00:00</t>
-  </si>
-  <si>
-    <t>808333f1c8668240</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.e271c1bb43^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_CERT_VAC_CT11_KO</t>
   </si>
   <si>
     <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>2023-06-06T14:32:46+00:00</t>
-  </si>
-  <si>
-    <t>dd9d6f873d3f4efe</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.0b92872779^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_CERT_VAC_CT12_KO</t>
@@ -1189,15 +1078,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-06-06T14:33:21+00:00</t>
-  </si>
-  <si>
-    <t>6c369f97af511f4e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.bc40f9c721^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_CERT_VAC_CT13_KO</t>
   </si>
   <si>
@@ -1206,15 +1086,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-06-06T14:33:49+00:00</t>
-  </si>
-  <si>
-    <t>4ab13c36a7bf7b1c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.0ee023f578^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_CERT_VAC_CT14_KO</t>
   </si>
   <si>
@@ -1223,29 +1094,11 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-06-06T14:34:26+00:00</t>
-  </si>
-  <si>
-    <t>cec556b1cb132542</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.0e41728773^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_CERT_VAC_CT15_KO</t>
   </si>
   <si>
     <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>2023-06-06T14:34:51+00:00</t>
-  </si>
-  <si>
-    <t>56f036f42037c159</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.594b34f52a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_CERT_VAC_CT16_KO</t>
@@ -1256,15 +1109,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-06-06T14:35:31+00:00</t>
-  </si>
-  <si>
-    <t>ff81a15438f56572</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.e9567b2448^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_CERT_VAC_CT17_KO</t>
   </si>
   <si>
@@ -1273,15 +1117,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-06-06T14:36:02+00:00</t>
-  </si>
-  <si>
-    <t>8af51512c2e88b9c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.09b38861ca^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_CERT_VAC_CT0</t>
   </si>
   <si>
@@ -1290,13 +1125,178 @@
 Il Documento CDA2 Certificato Vaccinale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 0" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-06-15T06:54:18+00:00</t>
-  </si>
-  <si>
-    <t>de722e732d8a610e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.b22926dcf3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-07-21T07:06:30+00:00</t>
+  </si>
+  <si>
+    <t>2023-07-21T07:07:08+00:00</t>
+  </si>
+  <si>
+    <t>2023-07-21T07:07:46+00:00</t>
+  </si>
+  <si>
+    <t>2023-07-21T07:08:22+00:00</t>
+  </si>
+  <si>
+    <t>2023-07-21T07:15:39+00:00</t>
+  </si>
+  <si>
+    <t>2023-07-21T07:17:43+00:00</t>
+  </si>
+  <si>
+    <t>2023-07-21T07:22:09+00:00</t>
+  </si>
+  <si>
+    <t>2023-07-21T07:20:17+00:00</t>
+  </si>
+  <si>
+    <t>2023-07-21T07:35:46+00:00</t>
+  </si>
+  <si>
+    <t>2023-07-21T07:36:36+00:00</t>
+  </si>
+  <si>
+    <t>2023-07-21T07:37:10+00:00</t>
+  </si>
+  <si>
+    <t>2023-07-21T07:37:48+00:00</t>
+  </si>
+  <si>
+    <t>2023-07-21T07:38:19+00:00</t>
+  </si>
+  <si>
+    <t>2023-07-21T07:38:45+00:00</t>
+  </si>
+  <si>
+    <t>2023-07-21T07:39:20+00:00</t>
+  </si>
+  <si>
+    <t>2023-07-21T07:41:01+00:00</t>
+  </si>
+  <si>
+    <t>2023-07-21T07:41:34+00:00</t>
+  </si>
+  <si>
+    <t>2023-07-21T07:42:06+00:00</t>
+  </si>
+  <si>
+    <t>2023-07-21T07:42:39+00:00</t>
+  </si>
+  <si>
+    <t>2023-07-21T07:06:03+00:00</t>
+  </si>
+  <si>
+    <t>8f7bc8a1bc5b6af5</t>
+  </si>
+  <si>
+    <t>1801a42467fe0a3d</t>
+  </si>
+  <si>
+    <t>9555162ccd4a84c9</t>
+  </si>
+  <si>
+    <t>427e1723e475f760</t>
+  </si>
+  <si>
+    <t>faf999d9bba9c0d0</t>
+  </si>
+  <si>
+    <t>63c217c1b06469c2</t>
+  </si>
+  <si>
+    <t>878102c525c5b96c</t>
+  </si>
+  <si>
+    <t>9443a80a0e24fec5</t>
+  </si>
+  <si>
+    <t>9b1d1524005bab72</t>
+  </si>
+  <si>
+    <t>b5ffcae2e3f5cbea</t>
+  </si>
+  <si>
+    <t>8a9f192092792587</t>
+  </si>
+  <si>
+    <t>647060b68dade075</t>
+  </si>
+  <si>
+    <t>cdb0c13012abc728</t>
+  </si>
+  <si>
+    <t>9e552d7c5818d62f</t>
+  </si>
+  <si>
+    <t>faabf5c4719396ee</t>
+  </si>
+  <si>
+    <t>d64fea4eba6087c7</t>
+  </si>
+  <si>
+    <t>961ff743807acbe7</t>
+  </si>
+  <si>
+    <t>4a14a0945dafcdc2</t>
+  </si>
+  <si>
+    <t>0135efcacfba2183</t>
+  </si>
+  <si>
+    <t>6f3ee0ab0cede03b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.80a5c4c0bf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.29f61d43b9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.2f85130319^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.9841e40b02^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.74592453c8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.a368d729d4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.0a8071ea3f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.6b441e0676^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.3b5ebb0469^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.8784c27dc4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.f0df7c28f3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.edbd3063de^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.169570471f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.b309a0bb68^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.0be2fd88a5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.335bfd2360^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.a6db9e9e04^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.701188e0fb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -4202,10 +4202,10 @@
   <dimension ref="A1:T629"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
+      <selection pane="bottomRight" activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5680,13 +5680,13 @@
         <v>45083</v>
       </c>
       <c r="G33" s="24" t="s">
-        <v>236</v>
+        <v>273</v>
       </c>
       <c r="H33" s="24" t="s">
-        <v>237</v>
+        <v>293</v>
       </c>
       <c r="I33" s="24" t="s">
-        <v>238</v>
+        <v>313</v>
       </c>
       <c r="J33" s="25" t="s">
         <v>68</v>
@@ -5717,22 +5717,22 @@
         <v>49</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F34" s="23">
         <v>45083</v>
       </c>
       <c r="G34" s="24" t="s">
-        <v>241</v>
+        <v>274</v>
       </c>
       <c r="H34" s="24" t="s">
-        <v>242</v>
+        <v>294</v>
       </c>
       <c r="I34" s="24" t="s">
-        <v>243</v>
+        <v>314</v>
       </c>
       <c r="J34" s="25" t="s">
         <v>68</v>
@@ -5763,22 +5763,22 @@
         <v>49</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="F35" s="23">
         <v>45083</v>
       </c>
       <c r="G35" s="24" t="s">
-        <v>246</v>
+        <v>275</v>
       </c>
       <c r="H35" s="24" t="s">
-        <v>247</v>
+        <v>295</v>
       </c>
       <c r="I35" s="24" t="s">
-        <v>248</v>
+        <v>315</v>
       </c>
       <c r="J35" s="25" t="s">
         <v>68</v>
@@ -5809,22 +5809,22 @@
         <v>49</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="F36" s="23">
         <v>45083</v>
       </c>
       <c r="G36" s="24" t="s">
-        <v>251</v>
+        <v>276</v>
       </c>
       <c r="H36" s="24" t="s">
-        <v>252</v>
+        <v>296</v>
       </c>
       <c r="I36" s="24" t="s">
-        <v>253</v>
+        <v>316</v>
       </c>
       <c r="J36" s="25" t="s">
         <v>68</v>
@@ -5855,7 +5855,7 @@
         <v>49</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="E37" s="22" t="s">
         <v>64</v>
@@ -5864,10 +5864,10 @@
         <v>45083</v>
       </c>
       <c r="G37" s="24" t="s">
-        <v>255</v>
+        <v>277</v>
       </c>
       <c r="H37" s="24" t="s">
-        <v>256</v>
+        <v>297</v>
       </c>
       <c r="I37" s="24" t="s">
         <v>212</v>
@@ -5909,7 +5909,7 @@
         <v>49</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="E38" s="22" t="s">
         <v>66</v>
@@ -5918,10 +5918,10 @@
         <v>45083</v>
       </c>
       <c r="G38" s="24" t="s">
-        <v>258</v>
+        <v>278</v>
       </c>
       <c r="H38" s="24" t="s">
-        <v>259</v>
+        <v>298</v>
       </c>
       <c r="I38" s="24" t="s">
         <v>212</v>
@@ -5963,7 +5963,7 @@
         <v>49</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
       <c r="E39" s="22" t="s">
         <v>67</v>
@@ -6019,22 +6019,22 @@
         <v>49</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
       <c r="F40" s="23">
         <v>45083</v>
       </c>
       <c r="G40" s="24" t="s">
-        <v>263</v>
+        <v>279</v>
       </c>
       <c r="H40" s="24" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="I40" s="24" t="s">
-        <v>265</v>
+        <v>317</v>
       </c>
       <c r="J40" s="25" t="s">
         <v>68</v>
@@ -6073,22 +6073,22 @@
         <v>49</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>266</v>
+        <v>247</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="F41" s="23">
         <v>45083</v>
       </c>
       <c r="G41" s="24" t="s">
-        <v>268</v>
+        <v>280</v>
       </c>
       <c r="H41" s="24" t="s">
-        <v>269</v>
+        <v>300</v>
       </c>
       <c r="I41" s="24" t="s">
-        <v>270</v>
+        <v>318</v>
       </c>
       <c r="J41" s="25" t="s">
         <v>68</v>
@@ -6127,22 +6127,22 @@
         <v>49</v>
       </c>
       <c r="D42" s="21" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
       <c r="F42" s="23">
         <v>45083</v>
       </c>
       <c r="G42" s="24" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="H42" s="24" t="s">
-        <v>274</v>
+        <v>301</v>
       </c>
       <c r="I42" s="24" t="s">
-        <v>275</v>
+        <v>319</v>
       </c>
       <c r="J42" s="25" t="s">
         <v>68</v>
@@ -6181,22 +6181,22 @@
         <v>49</v>
       </c>
       <c r="D43" s="21" t="s">
-        <v>276</v>
+        <v>251</v>
       </c>
       <c r="E43" s="22" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
       <c r="F43" s="23">
         <v>45083</v>
       </c>
       <c r="G43" s="24" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="H43" s="24" t="s">
-        <v>279</v>
+        <v>302</v>
       </c>
       <c r="I43" s="24" t="s">
-        <v>280</v>
+        <v>320</v>
       </c>
       <c r="J43" s="25" t="s">
         <v>68</v>
@@ -6235,10 +6235,10 @@
         <v>49</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>281</v>
+        <v>253</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>282</v>
+        <v>254</v>
       </c>
       <c r="F44" s="23">
         <v>45083</v>
@@ -6247,10 +6247,10 @@
         <v>283</v>
       </c>
       <c r="H44" s="24" t="s">
-        <v>284</v>
+        <v>303</v>
       </c>
       <c r="I44" s="24" t="s">
-        <v>285</v>
+        <v>321</v>
       </c>
       <c r="J44" s="25" t="s">
         <v>68</v>
@@ -6289,22 +6289,22 @@
         <v>49</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>286</v>
+        <v>255</v>
       </c>
       <c r="E45" s="22" t="s">
-        <v>287</v>
+        <v>256</v>
       </c>
       <c r="F45" s="23">
         <v>45083</v>
       </c>
       <c r="G45" s="24" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="H45" s="24" t="s">
-        <v>289</v>
+        <v>304</v>
       </c>
       <c r="I45" s="24" t="s">
-        <v>290</v>
+        <v>322</v>
       </c>
       <c r="J45" s="25" t="s">
         <v>68</v>
@@ -6343,22 +6343,22 @@
         <v>49</v>
       </c>
       <c r="D46" s="21" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>292</v>
+        <v>258</v>
       </c>
       <c r="F46" s="23">
         <v>45083</v>
       </c>
       <c r="G46" s="24" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="H46" s="24" t="s">
-        <v>294</v>
+        <v>305</v>
       </c>
       <c r="I46" s="24" t="s">
-        <v>295</v>
+        <v>323</v>
       </c>
       <c r="J46" s="25" t="s">
         <v>68</v>
@@ -6397,22 +6397,22 @@
         <v>49</v>
       </c>
       <c r="D47" s="21" t="s">
-        <v>296</v>
+        <v>259</v>
       </c>
       <c r="E47" s="22" t="s">
-        <v>297</v>
+        <v>260</v>
       </c>
       <c r="F47" s="23">
         <v>45083</v>
       </c>
       <c r="G47" s="24" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="H47" s="24" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
       <c r="I47" s="24" t="s">
-        <v>300</v>
+        <v>324</v>
       </c>
       <c r="J47" s="25" t="s">
         <v>68</v>
@@ -6451,22 +6451,22 @@
         <v>49</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>301</v>
+        <v>261</v>
       </c>
       <c r="E48" s="22" t="s">
-        <v>302</v>
+        <v>262</v>
       </c>
       <c r="F48" s="23">
         <v>45083</v>
       </c>
       <c r="G48" s="24" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
       <c r="H48" s="24" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="I48" s="24" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
       <c r="J48" s="25" t="s">
         <v>68</v>
@@ -6505,22 +6505,22 @@
         <v>49</v>
       </c>
       <c r="D49" s="21" t="s">
-        <v>306</v>
+        <v>263</v>
       </c>
       <c r="E49" s="22" t="s">
-        <v>307</v>
+        <v>264</v>
       </c>
       <c r="F49" s="23">
         <v>45083</v>
       </c>
       <c r="G49" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="H49" s="24" t="s">
         <v>308</v>
       </c>
-      <c r="H49" s="24" t="s">
-        <v>309</v>
-      </c>
       <c r="I49" s="24" t="s">
-        <v>310</v>
+        <v>326</v>
       </c>
       <c r="J49" s="25" t="s">
         <v>68</v>
@@ -6559,22 +6559,22 @@
         <v>49</v>
       </c>
       <c r="D50" s="21" t="s">
-        <v>311</v>
+        <v>265</v>
       </c>
       <c r="E50" s="22" t="s">
-        <v>312</v>
+        <v>266</v>
       </c>
       <c r="F50" s="23">
         <v>45083</v>
       </c>
       <c r="G50" s="24" t="s">
-        <v>313</v>
+        <v>289</v>
       </c>
       <c r="H50" s="24" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="I50" s="24" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="J50" s="25" t="s">
         <v>68</v>
@@ -6613,22 +6613,22 @@
         <v>49</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>316</v>
+        <v>267</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>317</v>
+        <v>268</v>
       </c>
       <c r="F51" s="23">
         <v>45083</v>
       </c>
       <c r="G51" s="24" t="s">
-        <v>318</v>
+        <v>290</v>
       </c>
       <c r="H51" s="24" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="I51" s="24" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="J51" s="25" t="s">
         <v>68</v>
@@ -6667,22 +6667,22 @@
         <v>49</v>
       </c>
       <c r="D52" s="21" t="s">
-        <v>321</v>
+        <v>269</v>
       </c>
       <c r="E52" s="22" t="s">
-        <v>322</v>
+        <v>270</v>
       </c>
       <c r="F52" s="23">
         <v>45083</v>
       </c>
       <c r="G52" s="24" t="s">
-        <v>323</v>
+        <v>291</v>
       </c>
       <c r="H52" s="24" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
       <c r="I52" s="24" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="J52" s="25" t="s">
         <v>68</v>
@@ -6721,19 +6721,19 @@
         <v>49</v>
       </c>
       <c r="D53" s="21" t="s">
-        <v>326</v>
+        <v>271</v>
       </c>
       <c r="E53" s="22" t="s">
-        <v>327</v>
+        <v>272</v>
       </c>
       <c r="F53" s="23">
         <v>45092</v>
       </c>
       <c r="G53" s="24" t="s">
-        <v>328</v>
+        <v>292</v>
       </c>
       <c r="H53" s="34" t="s">
-        <v>329</v>
+        <v>312</v>
       </c>
       <c r="I53" s="24" t="s">
         <v>330</v>

</xml_diff>